<commit_message>
added sem7 and done RK2 for economics
</commit_message>
<xml_diff>
--- a/Экономика/ДЗ Задачи Канторовича Эк ч1 2022/ДЗ Зад Канторовича Экон ч1 2022(студ).xlsx
+++ b/Экономика/ДЗ Задачи Канторовича Эк ч1 2022/ДЗ Зад Канторовича Экон ч1 2022(студ).xlsx
@@ -1,63 +1,137 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Viktor\Desktop\Карман\ДЗ Задачи Канторовича Эк ч1 2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Учёба\7 Семестр\Экономика\ДЗ Задачи Канторовича Эк ч1 2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8115A9-40D2-4CBA-A010-E9D694DC3EBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="108" windowWidth="9372" windowHeight="5220" tabRatio="828"/>
-    <workbookView visibility="hidden" xWindow="360" yWindow="300" windowWidth="9132" windowHeight="5028" firstSheet="5" activeTab="7"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="828" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="hidden" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="7" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF01000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ТитЛист" sheetId="1" r:id="rId1"/>
     <sheet name="Задание" sheetId="1099" r:id="rId2"/>
     <sheet name="Образец ДЗ" sheetId="3389" r:id="rId3"/>
-    <sheet name="ПонятиеОптимальности" sheetId="3396" r:id="rId4"/>
-    <sheet name="Оптимизатор" sheetId="3" r:id="rId5"/>
-    <sheet name="ПримерНастройкиПоиска" sheetId="3397" r:id="rId6"/>
-    <sheet name="Цвета" sheetId="3385" r:id="rId7"/>
-    <sheet name="ФакультативноОптимизатор2" sheetId="1085" r:id="rId8"/>
+    <sheet name="ДЗ" sheetId="3399" r:id="rId4"/>
+    <sheet name="РК2" sheetId="3400" r:id="rId5"/>
+    <sheet name="ПонятиеОптимальности" sheetId="3396" r:id="rId6"/>
+    <sheet name="Оптимизатор" sheetId="3" r:id="rId7"/>
+    <sheet name="ПримерНастройкиПоиска" sheetId="3397" r:id="rId8"/>
+    <sheet name="Цвета" sheetId="3385" r:id="rId9"/>
+    <sheet name="ФакультативноОптимизатор2" sheetId="1085" r:id="rId10"/>
   </sheets>
   <definedNames>
+    <definedName name="solver_adj" localSheetId="3" hidden="1">ДЗ!$B$8:$D$8</definedName>
+    <definedName name="solver_adj" localSheetId="4" hidden="1">РК2!$B$8:$D$8</definedName>
+    <definedName name="solver_cvg" localSheetId="3" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="2" hidden="1">"0.0001"</definedName>
+    <definedName name="solver_cvg" localSheetId="4" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="3" hidden="1">ДЗ!$F$11:$F$14</definedName>
+    <definedName name="solver_lhs1" localSheetId="4" hidden="1">РК2!$F$11:$F$14</definedName>
+    <definedName name="solver_mip" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="3" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="4" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="3" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="2" hidden="1">"0.075"</definedName>
+    <definedName name="solver_mrt" localSheetId="4" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_num" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_num" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="3" hidden="1">ДЗ!$C$17</definedName>
     <definedName name="solver_opt" localSheetId="2" hidden="1">'Образец ДЗ'!$N$30</definedName>
+    <definedName name="solver_opt" localSheetId="4" hidden="1">РК2!$C$17</definedName>
+    <definedName name="solver_pre" localSheetId="3" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="2" hidden="1">"0.000001"</definedName>
+    <definedName name="solver_pre" localSheetId="4" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_rel1" localSheetId="3" hidden="1">3</definedName>
+    <definedName name="solver_rel1" localSheetId="4" hidden="1">3</definedName>
+    <definedName name="solver_rhs1" localSheetId="3" hidden="1">ДЗ!$F$2:$F$5</definedName>
+    <definedName name="solver_rhs1" localSheetId="4" hidden="1">РК2!$F$2:$F$5</definedName>
+    <definedName name="solver_rlx" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="3" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="4" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="3" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="2" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="4" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
-    <definedName name="Область1" localSheetId="3">#REF!</definedName>
+    <definedName name="solver_ver" localSheetId="4" hidden="1">3</definedName>
+    <definedName name="Область1" localSheetId="5">#REF!</definedName>
     <definedName name="Область1">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="96">
   <si>
     <t>МГТУ им. Н.Э.Баумана</t>
   </si>
@@ -678,12 +752,103 @@
       <t>, можно прослеживать шаги поиска в многомерном пространстве.</t>
     </r>
   </si>
+  <si>
+    <t>ais</t>
+  </si>
+  <si>
+    <t>bi</t>
+  </si>
+  <si>
+    <t>Исходный ресурс</t>
+  </si>
+  <si>
+    <t>Полуфабрикаты</t>
+  </si>
+  <si>
+    <t>Трудовые ресурсы</t>
+  </si>
+  <si>
+    <t>Готовая продукция</t>
+  </si>
+  <si>
+    <t>Xs</t>
+  </si>
+  <si>
+    <t>sum ais xs</t>
+  </si>
+  <si>
+    <t>ais xs</t>
+  </si>
+  <si>
+    <t>критерий:</t>
+  </si>
+  <si>
+    <t>b1</t>
+  </si>
+  <si>
+    <t>x1</t>
+  </si>
+  <si>
+    <t>x2</t>
+  </si>
+  <si>
+    <t>x3</t>
+  </si>
+  <si>
+    <t>выпуск</t>
+  </si>
+  <si>
+    <t>Ограничивающий фактор</t>
+  </si>
+  <si>
+    <t>ИР</t>
+  </si>
+  <si>
+    <t>ТР</t>
+  </si>
+  <si>
+    <t>ТР и ИР</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>Модель</t>
+  </si>
+  <si>
+    <t>Эксперимент</t>
+  </si>
+  <si>
+    <t>Линейный выпуск п/ф</t>
+  </si>
+  <si>
+    <t>Xi</t>
+  </si>
+  <si>
+    <t>Отклонение</t>
+  </si>
+  <si>
+    <t>Сумма квадратов откл</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+    <numFmt numFmtId="169" formatCode="0.000000"/>
+  </numFmts>
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial Cyr"/>
@@ -751,6 +916,14 @@
     <font>
       <sz val="14"/>
       <name val="Arial Cyr"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -889,7 +1062,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -945,6 +1118,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -960,6 +1139,1026 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.2844054870499682E-2"/>
+          <c:y val="6.7940552016985137E-2"/>
+          <c:w val="0.89592503767217779"/>
+          <c:h val="0.85478442583212133"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Модель</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>РК2!$J$4:$T$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.90249999999970743</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5999999999997705</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.1520833333333078</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.6066666666668317</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.0000000000002491</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.3566666666668592</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.689583333333359</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.9999999999998348</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.2774999999997707</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.5000000000000435</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1DEE-4677-B082-80EEC85AA6F5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>РК2!$I$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Линейный выпуск п/ф</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>РК2!$J$6:$T$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-1DEE-4677-B082-80EEC85AA6F5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>РК2!$I$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Эксперимент</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>РК2!$J$5:$T$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-1DEE-4677-B082-80EEC85AA6F5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="539732063"/>
+        <c:axId val="539720831"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="539732063"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="539720831"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="539720831"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.000000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="539732063"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10324012427873942"/>
+          <c:y val="3.7006873505487786E-2"/>
+          <c:w val="0.25539280958721705"/>
+          <c:h val="0.21442335591151487"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -979,7 +2178,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="66" name="Рисунок 65"/>
+        <xdr:cNvPr id="66" name="Рисунок 65">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000042000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1026,6 +2231,47 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>464820</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>87630</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>579120</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Диаграмма 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8EB20789-17E7-46BC-87E2-E59A7056801E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>308610</xdr:colOff>
       <xdr:row>6</xdr:row>
@@ -1039,7 +2285,13 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="16" name="Группа 15"/>
+        <xdr:cNvPr id="16" name="Группа 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000010000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
@@ -1052,7 +2304,13 @@
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="2" name="Прямоугольник 1"/>
+          <xdr:cNvPr id="2" name="Прямоугольник 1">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
@@ -1074,7 +2332,6 @@
             <a:tailEnd type="none" w="med" len="med"/>
           </a:ln>
           <a:effectLst/>
-          <a:extLst/>
         </xdr:spPr>
         <xdr:txBody>
           <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t" upright="1"/>
@@ -1087,7 +2344,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="3" name="Дуга 2"/>
+          <xdr:cNvPr id="3" name="Дуга 2">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
@@ -1137,7 +2400,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="4" name="TextBox 3"/>
+          <xdr:cNvPr id="4" name="TextBox 3">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr txBox="1"/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -1182,7 +2451,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="5" name="Овал 4"/>
+          <xdr:cNvPr id="5" name="Овал 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000005000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
@@ -1206,7 +2481,6 @@
             <a:tailEnd type="none" w="med" len="med"/>
           </a:ln>
           <a:effectLst/>
-          <a:extLst/>
         </xdr:spPr>
         <xdr:txBody>
           <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t" upright="1"/>
@@ -1219,7 +2493,13 @@
       </xdr:sp>
       <xdr:cxnSp macro="">
         <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="7" name="Прямая соединительная линия 6"/>
+          <xdr:cNvPr id="7" name="Прямая соединительная линия 6">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000007000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvCxnSpPr/>
         </xdr:nvCxnSpPr>
         <xdr:spPr bwMode="auto">
@@ -1258,7 +2538,13 @@
       </xdr:cxnSp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="15" name="Овал 14"/>
+          <xdr:cNvPr id="15" name="Овал 14">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000F000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
@@ -1282,7 +2568,6 @@
             <a:tailEnd type="none" w="med" len="med"/>
           </a:ln>
           <a:effectLst/>
-          <a:extLst/>
         </xdr:spPr>
         <xdr:txBody>
           <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t" upright="1"/>
@@ -1311,7 +2596,13 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="31" name="Группа 30"/>
+        <xdr:cNvPr id="31" name="Группа 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
@@ -1324,7 +2615,13 @@
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="20" name="TextBox 19"/>
+          <xdr:cNvPr id="20" name="TextBox 19">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000014000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr txBox="1"/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -1369,7 +2666,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="18" name="Прямоугольник 17"/>
+          <xdr:cNvPr id="18" name="Прямоугольник 17">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000012000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
@@ -1391,7 +2694,6 @@
             <a:tailEnd type="none" w="med" len="med"/>
           </a:ln>
           <a:effectLst/>
-          <a:extLst/>
         </xdr:spPr>
         <xdr:txBody>
           <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t" upright="1"/>
@@ -1404,7 +2706,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="19" name="Дуга 18"/>
+          <xdr:cNvPr id="19" name="Дуга 18">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000013000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
@@ -1454,7 +2762,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="21" name="Овал 20"/>
+          <xdr:cNvPr id="21" name="Овал 20">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000015000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
@@ -1478,7 +2792,6 @@
             <a:tailEnd type="none" w="med" len="med"/>
           </a:ln>
           <a:effectLst/>
-          <a:extLst/>
         </xdr:spPr>
         <xdr:txBody>
           <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t" upright="1"/>
@@ -1491,7 +2804,13 @@
       </xdr:sp>
       <xdr:cxnSp macro="">
         <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="22" name="Прямая соединительная линия 21"/>
+          <xdr:cNvPr id="22" name="Прямая соединительная линия 21">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000016000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvCxnSpPr/>
         </xdr:nvCxnSpPr>
         <xdr:spPr bwMode="auto">
@@ -1530,7 +2849,13 @@
       </xdr:cxnSp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="23" name="Овал 22"/>
+          <xdr:cNvPr id="23" name="Овал 22">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000017000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
@@ -1554,7 +2879,6 @@
             <a:tailEnd type="none" w="med" len="med"/>
           </a:ln>
           <a:effectLst/>
-          <a:extLst/>
         </xdr:spPr>
         <xdr:txBody>
           <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t" upright="1"/>
@@ -1567,7 +2891,13 @@
       </xdr:sp>
       <xdr:cxnSp macro="">
         <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="25" name="Прямая соединительная линия 24"/>
+          <xdr:cNvPr id="25" name="Прямая соединительная линия 24">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000019000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvCxnSpPr/>
         </xdr:nvCxnSpPr>
         <xdr:spPr bwMode="auto">
@@ -1606,7 +2936,13 @@
       </xdr:cxnSp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="26" name="Дуга 25"/>
+          <xdr:cNvPr id="26" name="Дуга 25">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001A000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
@@ -1656,7 +2992,13 @@
       </xdr:sp>
       <xdr:cxnSp macro="">
         <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="27" name="Прямая соединительная линия 26"/>
+          <xdr:cNvPr id="27" name="Прямая соединительная линия 26">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001B000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvCxnSpPr/>
         </xdr:nvCxnSpPr>
         <xdr:spPr bwMode="auto">
@@ -1695,7 +3037,13 @@
       </xdr:cxnSp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="28" name="Овал 27"/>
+          <xdr:cNvPr id="28" name="Овал 27">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001C000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
@@ -1719,7 +3067,6 @@
             <a:tailEnd type="none" w="med" len="med"/>
           </a:ln>
           <a:effectLst/>
-          <a:extLst/>
         </xdr:spPr>
         <xdr:txBody>
           <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t" upright="1"/>
@@ -1732,7 +3079,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="29" name="Овал 28"/>
+          <xdr:cNvPr id="29" name="Овал 28">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001D000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
@@ -1756,7 +3109,6 @@
             <a:tailEnd type="none" w="med" len="med"/>
           </a:ln>
           <a:effectLst/>
-          <a:extLst/>
         </xdr:spPr>
         <xdr:txBody>
           <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t" upright="1"/>
@@ -1785,7 +3137,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="33" name="TextBox 32"/>
+        <xdr:cNvPr id="33" name="TextBox 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000021000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1845,7 +3203,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="34" name="Прямоугольник 33"/>
+        <xdr:cNvPr id="34" name="Прямоугольник 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000022000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -1867,7 +3231,6 @@
           <a:tailEnd type="none" w="med" len="med"/>
         </a:ln>
         <a:effectLst/>
-        <a:extLst/>
       </xdr:spPr>
       <xdr:txBody>
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t" upright="1"/>
@@ -1895,7 +3258,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="35" name="Дуга 34"/>
+        <xdr:cNvPr id="35" name="Дуга 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000023000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -1960,7 +3329,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="40" name="Дуга 39"/>
+        <xdr:cNvPr id="40" name="Дуга 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000028000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -2025,7 +3400,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="41" name="Прямая соединительная линия 40"/>
+        <xdr:cNvPr id="41" name="Прямая соединительная линия 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000029000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr bwMode="auto">
@@ -2079,7 +3460,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="42" name="Овал 41"/>
+        <xdr:cNvPr id="42" name="Овал 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00002A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -2103,7 +3490,6 @@
           <a:tailEnd type="none" w="med" len="med"/>
         </a:ln>
         <a:effectLst/>
-        <a:extLst/>
       </xdr:spPr>
       <xdr:txBody>
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t" upright="1"/>
@@ -2131,7 +3517,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="43" name="Овал 42"/>
+        <xdr:cNvPr id="43" name="Овал 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00002B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -2155,7 +3547,6 @@
           <a:tailEnd type="none" w="med" len="med"/>
         </a:ln>
         <a:effectLst/>
-        <a:extLst/>
       </xdr:spPr>
       <xdr:txBody>
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t" upright="1"/>
@@ -2183,7 +3574,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="47" name="Дуга 46"/>
+        <xdr:cNvPr id="47" name="Дуга 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00002F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -2248,7 +3645,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="48" name="Дуга 47"/>
+        <xdr:cNvPr id="48" name="Дуга 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000030000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -2313,7 +3716,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="49" name="Дуга 48"/>
+        <xdr:cNvPr id="49" name="Дуга 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000031000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -2378,7 +3787,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="50" name="Дуга 49"/>
+        <xdr:cNvPr id="50" name="Дуга 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000032000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -2443,7 +3858,13 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="46" name="Группа 45"/>
+        <xdr:cNvPr id="46" name="Группа 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00002E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
@@ -2456,7 +3877,13 @@
       </xdr:grpSpPr>
       <xdr:cxnSp macro="">
         <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="37" name="Прямая соединительная линия 36"/>
+          <xdr:cNvPr id="37" name="Прямая соединительная линия 36">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000025000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvCxnSpPr/>
         </xdr:nvCxnSpPr>
         <xdr:spPr bwMode="auto">
@@ -2495,7 +3922,13 @@
       </xdr:cxnSp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="38" name="Овал 37"/>
+          <xdr:cNvPr id="38" name="Овал 37">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000026000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
@@ -2519,7 +3952,6 @@
             <a:tailEnd type="none" w="med" len="med"/>
           </a:ln>
           <a:effectLst/>
-          <a:extLst/>
         </xdr:spPr>
         <xdr:txBody>
           <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t" upright="1"/>
@@ -2532,7 +3964,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="44" name="Овал 43"/>
+          <xdr:cNvPr id="44" name="Овал 43">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00002C000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr bwMode="auto">
@@ -2556,7 +3994,6 @@
             <a:tailEnd type="none" w="med" len="med"/>
           </a:ln>
           <a:effectLst/>
-          <a:extLst/>
         </xdr:spPr>
         <xdr:txBody>
           <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t" upright="1"/>
@@ -2573,7 +4010,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2590,7 +4027,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Рисунок 4"/>
+        <xdr:cNvPr id="5" name="Рисунок 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2616,7 +4059,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2633,7 +4076,13 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="7290" name="Group 25"/>
+        <xdr:cNvPr id="7290" name="Group 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-00007A1C0000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGrpSpPr>
           <a:grpSpLocks/>
         </xdr:cNvGrpSpPr>
@@ -2648,7 +4097,13 @@
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="7173" name="Text Box 5"/>
+          <xdr:cNvPr id="7173" name="Text Box 5">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-0000051C0000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr txBox="1">
             <a:spLocks noChangeArrowheads="1"/>
           </xdr:cNvSpPr>
@@ -2717,7 +4172,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="7184" name="Text Box 16"/>
+          <xdr:cNvPr id="7184" name="Text Box 16">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-0000101C0000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr txBox="1">
             <a:spLocks noChangeArrowheads="1"/>
           </xdr:cNvSpPr>
@@ -2786,7 +4247,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="7293" name="Line 1"/>
+          <xdr:cNvPr id="7293" name="Line 1">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-00007D1C0000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks noChangeShapeType="1"/>
           </xdr:cNvSpPr>
@@ -2829,7 +4296,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="7294" name="Line 2"/>
+          <xdr:cNvPr id="7294" name="Line 2">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-00007E1C0000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks noChangeShapeType="1"/>
           </xdr:cNvSpPr>
@@ -2872,7 +4345,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="7295" name="Line 3"/>
+          <xdr:cNvPr id="7295" name="Line 3">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-00007F1C0000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks noChangeShapeType="1"/>
           </xdr:cNvSpPr>
@@ -2915,7 +4394,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="7174" name="Text Box 6"/>
+          <xdr:cNvPr id="7174" name="Text Box 6">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-0000061C0000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr txBox="1">
             <a:spLocks noChangeArrowheads="1"/>
           </xdr:cNvSpPr>
@@ -2984,7 +4469,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="7297" name="Line 7"/>
+          <xdr:cNvPr id="7297" name="Line 7">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-0000811C0000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks noChangeShapeType="1"/>
           </xdr:cNvSpPr>
@@ -3027,7 +4518,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="7298" name="Line 8"/>
+          <xdr:cNvPr id="7298" name="Line 8">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-0000821C0000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks noChangeShapeType="1"/>
           </xdr:cNvSpPr>
@@ -3070,7 +4567,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="7299" name="Line 9"/>
+          <xdr:cNvPr id="7299" name="Line 9">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-0000831C0000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks noChangeShapeType="1"/>
           </xdr:cNvSpPr>
@@ -3113,7 +4616,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="7300" name="Line 10"/>
+          <xdr:cNvPr id="7300" name="Line 10">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-0000841C0000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks noChangeShapeType="1"/>
           </xdr:cNvSpPr>
@@ -3157,7 +4666,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="7179" name="Text Box 11"/>
+          <xdr:cNvPr id="7179" name="Text Box 11">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-00000B1C0000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr txBox="1">
             <a:spLocks noChangeArrowheads="1"/>
           </xdr:cNvSpPr>
@@ -3226,7 +4741,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="7302" name="Line 12"/>
+          <xdr:cNvPr id="7302" name="Line 12">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-0000861C0000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks noChangeShapeType="1"/>
           </xdr:cNvSpPr>
@@ -3269,7 +4790,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="7303" name="Line 13"/>
+          <xdr:cNvPr id="7303" name="Line 13">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-0000871C0000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks noChangeShapeType="1"/>
           </xdr:cNvSpPr>
@@ -3313,7 +4840,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="7182" name="Text Box 14"/>
+          <xdr:cNvPr id="7182" name="Text Box 14">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-00000E1C0000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr txBox="1">
             <a:spLocks noChangeArrowheads="1"/>
           </xdr:cNvSpPr>
@@ -3382,7 +4915,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="7183" name="Text Box 15"/>
+          <xdr:cNvPr id="7183" name="Text Box 15">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-00000F1C0000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr txBox="1">
             <a:spLocks noChangeArrowheads="1"/>
           </xdr:cNvSpPr>
@@ -3451,7 +4990,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="7306" name="Line 17"/>
+          <xdr:cNvPr id="7306" name="Line 17">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-00008A1C0000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks noChangeShapeType="1"/>
           </xdr:cNvSpPr>
@@ -3495,7 +5040,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="7186" name="Text Box 18"/>
+          <xdr:cNvPr id="7186" name="Text Box 18">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-0000121C0000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr txBox="1">
             <a:spLocks noChangeArrowheads="1"/>
           </xdr:cNvSpPr>
@@ -3564,7 +5115,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="7308" name="Line 19"/>
+          <xdr:cNvPr id="7308" name="Line 19">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-00008C1C0000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks noChangeShapeType="1"/>
           </xdr:cNvSpPr>
@@ -3607,7 +5164,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="7309" name="Line 20"/>
+          <xdr:cNvPr id="7309" name="Line 20">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-00008D1C0000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks noChangeShapeType="1"/>
           </xdr:cNvSpPr>
@@ -3650,7 +5213,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="7310" name="Line 21"/>
+          <xdr:cNvPr id="7310" name="Line 21">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-00008E1C0000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr>
             <a:spLocks noChangeShapeType="1"/>
           </xdr:cNvSpPr>
@@ -3693,7 +5262,13 @@
       </xdr:sp>
       <xdr:grpSp>
         <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="7311" name="Group 23"/>
+          <xdr:cNvPr id="7311" name="Group 23">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-00008F1C0000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvGrpSpPr>
             <a:grpSpLocks/>
           </xdr:cNvGrpSpPr>
@@ -3708,7 +5283,13 @@
         </xdr:grpSpPr>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="7172" name="Text Box 4"/>
+            <xdr:cNvPr id="7172" name="Text Box 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-0000041C0000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvSpPr txBox="1">
               <a:spLocks noChangeArrowheads="1"/>
             </xdr:cNvSpPr>
@@ -3807,7 +5388,13 @@
         </xdr:sp>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="7313" name="AutoShape 22"/>
+            <xdr:cNvPr id="7313" name="AutoShape 22">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-0000911C0000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvSpPr>
               <a:spLocks/>
             </xdr:cNvSpPr>
@@ -4207,55 +5794,55 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="47.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="13.8" thickBot="1"/>
-    <row r="2" spans="2:4" ht="14.4" thickTop="1">
+    <row r="1" spans="2:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:4" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="2:4">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="2:4">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="2:4">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="2:4" ht="7.8" customHeight="1">
+    <row r="6" spans="2:4" ht="7.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
       <c r="D6" s="6"/>
     </row>
-    <row r="7" spans="2:4" ht="44.4" customHeight="1">
+    <row r="7" spans="2:4" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
       <c r="C7" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="2:4" ht="17.25" customHeight="1">
+    <row r="8" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
         <v>2</v>
       </c>
@@ -4264,46 +5851,46 @@
       </c>
       <c r="D8" s="9"/>
     </row>
-    <row r="9" spans="2:4" ht="11.25" customHeight="1">
+    <row r="9" spans="2:4" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="6"/>
     </row>
-    <row r="10" spans="2:4" ht="11.25" customHeight="1">
+    <row r="10" spans="2:4" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="4"/>
       <c r="C10" s="7"/>
       <c r="D10" s="9"/>
     </row>
-    <row r="11" spans="2:4" ht="15.6">
+    <row r="11" spans="2:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="B11" s="4"/>
       <c r="C11" s="7"/>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="2:4" ht="26.25" customHeight="1">
+    <row r="12" spans="2:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="4"/>
       <c r="C12" s="7"/>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="2:4" ht="21" customHeight="1">
+    <row r="13" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="4"/>
       <c r="C13" s="7"/>
       <c r="D13" s="6"/>
     </row>
-    <row r="14" spans="2:4" ht="15.6">
+    <row r="14" spans="2:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="B14" s="4"/>
       <c r="C14" s="7"/>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="2:4" ht="13.8" thickBot="1">
+    <row r="15" spans="2:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="10"/>
       <c r="C15" s="11" t="s">
         <v>37</v>
       </c>
       <c r="D15" s="12"/>
     </row>
-    <row r="16" spans="2:4" ht="16.2" thickTop="1">
+    <row r="16" spans="2:4" ht="16.2" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C16" s="13"/>
     </row>
   </sheetData>
@@ -4313,103 +5900,220 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="B1:B22"/>
+  <sheetViews>
+    <sheetView zoomScale="130" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="1.109375" customWidth="1"/>
+    <col min="2" max="2" width="81" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="14"/>
+    </row>
+    <row r="13" spans="2:2" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B16" s="14"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="14"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="14"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="14"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="14"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="14"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:B24"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A3" workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
     <col min="2" max="2" width="122.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="21" customHeight="1">
+    <row r="1" spans="2:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="25" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="2:2" ht="41.4" customHeight="1">
+    <row r="2" spans="2:2" ht="41.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="26" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="2:2" ht="12.75" customHeight="1">
+    <row r="3" spans="2:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="26"/>
     </row>
-    <row r="4" spans="2:2" ht="46.8" customHeight="1">
+    <row r="4" spans="2:2" ht="46.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="26" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="2:2" ht="15" customHeight="1">
+    <row r="5" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="26"/>
     </row>
-    <row r="6" spans="2:2" ht="52.2" customHeight="1">
+    <row r="6" spans="2:2" ht="52.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="26" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="15.6" customHeight="1">
+    <row r="7" spans="2:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="26"/>
     </row>
-    <row r="8" spans="2:2" ht="89.4" customHeight="1">
+    <row r="8" spans="2:2" ht="89.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="26" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="2:2" ht="17.399999999999999">
+    <row r="9" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="B9" s="26"/>
     </row>
-    <row r="10" spans="2:2" ht="88.2" customHeight="1">
+    <row r="10" spans="2:2" ht="88.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="26" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="2:2" ht="17.399999999999999">
+    <row r="11" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="B11" s="26"/>
     </row>
-    <row r="12" spans="2:2" ht="17.399999999999999">
+    <row r="12" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="B12" s="26"/>
     </row>
-    <row r="13" spans="2:2" ht="17.399999999999999">
+    <row r="13" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="B13" s="26"/>
     </row>
-    <row r="14" spans="2:2" ht="17.399999999999999">
+    <row r="14" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="B14" s="26"/>
     </row>
-    <row r="15" spans="2:2" ht="17.399999999999999">
+    <row r="15" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="B15" s="26"/>
     </row>
-    <row r="16" spans="2:2" ht="17.399999999999999">
+    <row r="16" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="B16" s="26"/>
     </row>
-    <row r="17" spans="2:2" ht="17.399999999999999">
+    <row r="17" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="B17" s="26"/>
     </row>
-    <row r="18" spans="2:2" ht="17.399999999999999">
+    <row r="18" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="B18" s="26"/>
     </row>
-    <row r="19" spans="2:2" ht="17.399999999999999">
+    <row r="19" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="B19" s="26"/>
     </row>
-    <row r="20" spans="2:2" ht="17.399999999999999">
+    <row r="20" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="B20" s="26"/>
     </row>
-    <row r="21" spans="2:2" ht="17.399999999999999">
+    <row r="21" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B21" s="27"/>
     </row>
-    <row r="22" spans="2:2" ht="17.399999999999999">
+    <row r="22" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B22" s="27"/>
     </row>
-    <row r="23" spans="2:2" ht="17.399999999999999">
+    <row r="23" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B23" s="27"/>
     </row>
-    <row r="24" spans="2:2" ht="17.399999999999999">
+    <row r="24" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B24" s="27"/>
     </row>
   </sheetData>
@@ -4419,15 +6123,15 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A11" workbookViewId="0">
       <selection activeCell="N30" sqref="N30"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4435,114 +6139,872 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F1EE2FF-EBCD-4694-A431-6C481B2809F7}">
+  <dimension ref="A1:N17"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="C1" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K1" t="s">
+        <v>79</v>
+      </c>
+      <c r="L1" t="s">
+        <v>80</v>
+      </c>
+      <c r="M1" t="s">
+        <v>81</v>
+      </c>
+      <c r="N1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="30">
+        <v>-1</v>
+      </c>
+      <c r="C2" s="30">
+        <v>0</v>
+      </c>
+      <c r="D2" s="30">
+        <v>0</v>
+      </c>
+      <c r="F2" s="30">
+        <v>-2</v>
+      </c>
+      <c r="I2" s="30">
+        <v>-1</v>
+      </c>
+      <c r="J2" s="32">
+        <v>1</v>
+      </c>
+      <c r="K2" s="32">
+        <v>0</v>
+      </c>
+      <c r="L2" s="32">
+        <v>1</v>
+      </c>
+      <c r="M2" s="31">
+        <v>2</v>
+      </c>
+      <c r="N2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="30">
+        <v>1</v>
+      </c>
+      <c r="C3" s="30">
+        <v>-1</v>
+      </c>
+      <c r="D3" s="30">
+        <v>-1</v>
+      </c>
+      <c r="F3" s="30">
+        <v>0</v>
+      </c>
+      <c r="I3" s="30">
+        <v>-2</v>
+      </c>
+      <c r="J3" s="32">
+        <v>2</v>
+      </c>
+      <c r="K3" s="32">
+        <v>1.3333333333333326</v>
+      </c>
+      <c r="L3" s="32">
+        <v>0.66666666666666707</v>
+      </c>
+      <c r="M3">
+        <v>2.67</v>
+      </c>
+      <c r="N3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="30">
+        <v>-1</v>
+      </c>
+      <c r="C4" s="30">
+        <v>-1</v>
+      </c>
+      <c r="D4" s="30">
+        <v>-4</v>
+      </c>
+      <c r="F4" s="30">
+        <v>-6</v>
+      </c>
+      <c r="I4" s="30">
+        <v>-3</v>
+      </c>
+      <c r="J4" s="32">
+        <v>3</v>
+      </c>
+      <c r="K4" s="32">
+        <v>2.9999999677141509</v>
+      </c>
+      <c r="L4" s="32">
+        <v>2.4835263105297644E-9</v>
+      </c>
+      <c r="M4" s="33">
+        <v>3</v>
+      </c>
+      <c r="N4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="30">
+        <v>0</v>
+      </c>
+      <c r="C5" s="30">
+        <v>1</v>
+      </c>
+      <c r="D5" s="30">
+        <v>2</v>
+      </c>
+      <c r="F5" s="30">
+        <v>0</v>
+      </c>
+      <c r="I5" s="30">
+        <v>-4</v>
+      </c>
+      <c r="J5" s="32">
+        <v>3</v>
+      </c>
+      <c r="K5" s="32">
+        <v>2.9999999677141509</v>
+      </c>
+      <c r="L5" s="32">
+        <v>2.4835263105297644E-9</v>
+      </c>
+      <c r="M5" s="33">
+        <v>3</v>
+      </c>
+      <c r="N5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="C7" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" s="29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="B8" s="32">
+        <v>1.9999999999999998</v>
+      </c>
+      <c r="C8" s="32">
+        <v>1.3333333673262586</v>
+      </c>
+      <c r="D8" s="32">
+        <v>0.66666665593205843</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="C10" s="29" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="B11" s="32">
+        <f>B2*$B$8</f>
+        <v>-1.9999999999999998</v>
+      </c>
+      <c r="C11" s="32">
+        <f>C2*$C$8</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="32">
+        <f>D2*$D$8</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="32">
+        <f>SUM(B11:D11)</f>
+        <v>-1.9999999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="B12" s="32">
+        <f>B3*$B$8</f>
+        <v>1.9999999999999998</v>
+      </c>
+      <c r="C12" s="32">
+        <f>C3*$C$8</f>
+        <v>-1.3333333673262586</v>
+      </c>
+      <c r="D12" s="32">
+        <f>D3*$D$8</f>
+        <v>-0.66666665593205843</v>
+      </c>
+      <c r="F12" s="32">
+        <f>SUM(B12:D12)</f>
+        <v>-2.3258317272123463E-8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="B13" s="32">
+        <f>B4*$B$8</f>
+        <v>-1.9999999999999998</v>
+      </c>
+      <c r="C13" s="32">
+        <f>C4*$C$8</f>
+        <v>-1.3333333673262586</v>
+      </c>
+      <c r="D13" s="32">
+        <f>D4*$D$8</f>
+        <v>-2.6666666237282337</v>
+      </c>
+      <c r="F13" s="32">
+        <f>SUM(B13:D13)</f>
+        <v>-5.9999999910544926</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="B14" s="32">
+        <f>B5*$B$8</f>
+        <v>0</v>
+      </c>
+      <c r="C14" s="32">
+        <f>C5*$C$8</f>
+        <v>1.3333333673262586</v>
+      </c>
+      <c r="D14" s="32">
+        <f>D5*$D$8</f>
+        <v>1.3333333118641169</v>
+      </c>
+      <c r="F14" s="32">
+        <f>SUM(B14:D14)</f>
+        <v>2.6666666791903753</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="B17" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" s="31">
+        <f>C14+D14</f>
+        <v>2.6666666791903753</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF0C9210-74A1-403A-895A-A134ACCC32CD}">
+  <dimension ref="A1:T23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.77734375" customWidth="1"/>
+    <col min="11" max="11" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="19" width="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="C1" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K1" t="s">
+        <v>87</v>
+      </c>
+      <c r="L1" t="s">
+        <v>88</v>
+      </c>
+      <c r="M1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="30">
+        <v>-1</v>
+      </c>
+      <c r="C2" s="30">
+        <v>0</v>
+      </c>
+      <c r="D2" s="30">
+        <v>0</v>
+      </c>
+      <c r="F2" s="30">
+        <v>-2</v>
+      </c>
+      <c r="J2" s="34">
+        <v>1.0277777777772206</v>
+      </c>
+      <c r="K2" s="34">
+        <v>-0.13763888888857576</v>
+      </c>
+      <c r="L2" s="34">
+        <v>1.2847222222171226E-2</v>
+      </c>
+      <c r="M2" s="34">
+        <v>-4.8611111110858127E-4</v>
+      </c>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+    </row>
+    <row r="3" spans="1:20" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="30">
+        <v>1</v>
+      </c>
+      <c r="C3" s="30">
+        <v>-1</v>
+      </c>
+      <c r="D3" s="30">
+        <v>-1</v>
+      </c>
+      <c r="F3" s="30">
+        <v>0</v>
+      </c>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="33"/>
+      <c r="P3" s="33"/>
+      <c r="Q3" s="33"/>
+      <c r="R3" s="33"/>
+      <c r="S3" s="33"/>
+      <c r="T3" s="33"/>
+    </row>
+    <row r="4" spans="1:20" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="30">
+        <v>-1</v>
+      </c>
+      <c r="C4" s="30">
+        <v>-1</v>
+      </c>
+      <c r="D4" s="30">
+        <v>-4</v>
+      </c>
+      <c r="F4" s="30">
+        <v>-6</v>
+      </c>
+      <c r="I4" t="s">
+        <v>90</v>
+      </c>
+      <c r="J4" s="34">
+        <f t="shared" ref="J4:T4" si="0">$J$2*J8+$K$2*J8^2+$L$2*J8^3+$M$2*J8^4</f>
+        <v>0</v>
+      </c>
+      <c r="K4" s="34">
+        <f t="shared" si="0"/>
+        <v>0.90249999999970743</v>
+      </c>
+      <c r="L4" s="34">
+        <f t="shared" si="0"/>
+        <v>1.5999999999997705</v>
+      </c>
+      <c r="M4" s="34">
+        <f t="shared" si="0"/>
+        <v>2.1520833333333078</v>
+      </c>
+      <c r="N4" s="34">
+        <f t="shared" si="0"/>
+        <v>2.6066666666668317</v>
+      </c>
+      <c r="O4" s="34">
+        <f t="shared" si="0"/>
+        <v>3.0000000000002491</v>
+      </c>
+      <c r="P4" s="34">
+        <f t="shared" si="0"/>
+        <v>3.3566666666668592</v>
+      </c>
+      <c r="Q4" s="34">
+        <f t="shared" si="0"/>
+        <v>3.689583333333359</v>
+      </c>
+      <c r="R4" s="34">
+        <f t="shared" si="0"/>
+        <v>3.9999999999998348</v>
+      </c>
+      <c r="S4" s="34">
+        <f t="shared" si="0"/>
+        <v>4.2774999999997707</v>
+      </c>
+      <c r="T4" s="34">
+        <f t="shared" si="0"/>
+        <v>4.5000000000000435</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="30">
+        <v>0</v>
+      </c>
+      <c r="C5" s="30">
+        <v>1</v>
+      </c>
+      <c r="D5" s="30">
+        <v>2</v>
+      </c>
+      <c r="F5" s="30">
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>91</v>
+      </c>
+      <c r="J5" s="33">
+        <v>0</v>
+      </c>
+      <c r="K5" s="33"/>
+      <c r="L5" s="33">
+        <v>1.6</v>
+      </c>
+      <c r="M5" s="33"/>
+      <c r="N5" s="33"/>
+      <c r="O5" s="33">
+        <v>3</v>
+      </c>
+      <c r="P5" s="33"/>
+      <c r="Q5" s="33"/>
+      <c r="R5" s="33">
+        <v>4</v>
+      </c>
+      <c r="S5" s="33"/>
+      <c r="T5" s="33">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>92</v>
+      </c>
+      <c r="J6" s="33">
+        <v>0</v>
+      </c>
+      <c r="K6" s="33">
+        <v>1</v>
+      </c>
+      <c r="L6" s="33">
+        <v>2</v>
+      </c>
+      <c r="M6" s="33">
+        <v>3</v>
+      </c>
+      <c r="N6" s="33">
+        <v>4</v>
+      </c>
+      <c r="O6" s="33">
+        <v>5</v>
+      </c>
+      <c r="P6" s="33">
+        <v>6</v>
+      </c>
+      <c r="Q6" s="33">
+        <v>7</v>
+      </c>
+      <c r="R6" s="33">
+        <v>8</v>
+      </c>
+      <c r="S6" s="33">
+        <v>9</v>
+      </c>
+      <c r="T6" s="33">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="C7" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="J7" s="33"/>
+      <c r="K7" s="33"/>
+      <c r="L7" s="33"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="33"/>
+      <c r="O7" s="33"/>
+      <c r="P7" s="33"/>
+      <c r="Q7" s="33"/>
+      <c r="R7" s="33"/>
+      <c r="S7" s="33"/>
+      <c r="T7" s="33"/>
+    </row>
+    <row r="8" spans="1:20" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="B8" s="32">
+        <v>2.7025602291954129</v>
+      </c>
+      <c r="C8" s="32">
+        <v>2.5042670826519471</v>
+      </c>
+      <c r="D8" s="32">
+        <v>0.19829316980178291</v>
+      </c>
+      <c r="I8" t="s">
+        <v>93</v>
+      </c>
+      <c r="J8" s="33">
+        <v>0</v>
+      </c>
+      <c r="K8" s="33">
+        <v>1</v>
+      </c>
+      <c r="L8" s="33">
+        <v>2</v>
+      </c>
+      <c r="M8" s="33">
+        <v>3</v>
+      </c>
+      <c r="N8" s="33">
+        <v>4</v>
+      </c>
+      <c r="O8" s="33">
+        <v>5</v>
+      </c>
+      <c r="P8" s="33">
+        <v>6</v>
+      </c>
+      <c r="Q8" s="33">
+        <v>7</v>
+      </c>
+      <c r="R8" s="33">
+        <v>8</v>
+      </c>
+      <c r="S8" s="33">
+        <v>9</v>
+      </c>
+      <c r="T8" s="33">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="J9" s="33"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="33"/>
+      <c r="N9" s="33"/>
+      <c r="O9" s="33"/>
+      <c r="P9" s="33"/>
+      <c r="Q9" s="33"/>
+      <c r="R9" s="33"/>
+      <c r="S9" s="33"/>
+      <c r="T9" s="33"/>
+    </row>
+    <row r="10" spans="1:20" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="C10" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="I10" t="s">
+        <v>94</v>
+      </c>
+      <c r="J10" s="34">
+        <f>(J4-J5)^2</f>
+        <v>0</v>
+      </c>
+      <c r="K10" s="34"/>
+      <c r="L10" s="34">
+        <f t="shared" ref="K10:T10" si="1">(L4-L5)^2</f>
+        <v>5.2713460623904756E-26</v>
+      </c>
+      <c r="M10" s="34"/>
+      <c r="N10" s="34"/>
+      <c r="O10" s="34">
+        <f t="shared" si="1"/>
+        <v>6.2067773238015514E-26</v>
+      </c>
+      <c r="P10" s="34"/>
+      <c r="Q10" s="34"/>
+      <c r="R10" s="34">
+        <f t="shared" si="1"/>
+        <v>2.7291431877026124E-26</v>
+      </c>
+      <c r="S10" s="34"/>
+      <c r="T10" s="34">
+        <f t="shared" si="1"/>
+        <v>1.8940550334356493E-27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="B11" s="32">
+        <f>B2*($J$2*B8+$K$2*B8^2+$L$2*B8^3+$M$2*B8^4)</f>
+        <v>-1.9999998925193252</v>
+      </c>
+      <c r="C11" s="32">
+        <f>C2*$C$8</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="32">
+        <f>D2*$D$8</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="32">
+        <f>SUM(B11:D11)</f>
+        <v>-1.9999998925193252</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="B12" s="32">
+        <f>B3*$B$8</f>
+        <v>2.7025602291954129</v>
+      </c>
+      <c r="C12" s="32">
+        <f>C3*$C$8</f>
+        <v>-2.5042670826519471</v>
+      </c>
+      <c r="D12" s="32">
+        <f>D3*$D$8</f>
+        <v>-0.19829316980178291</v>
+      </c>
+      <c r="F12" s="32">
+        <f>SUM(B12:D12)</f>
+        <v>-2.3258317050078858E-8</v>
+      </c>
+      <c r="I12" t="s">
+        <v>95</v>
+      </c>
+      <c r="J12" s="34">
+        <f>SUM(J10:T10)</f>
+        <v>1.4396672077238204E-25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="B13" s="32">
+        <f>B4*$B$8</f>
+        <v>-2.7025602291954129</v>
+      </c>
+      <c r="C13" s="32">
+        <f>C4*$C$8</f>
+        <v>-2.5042670826519471</v>
+      </c>
+      <c r="D13" s="32">
+        <f>D4*$D$8</f>
+        <v>-0.79317267920713164</v>
+      </c>
+      <c r="F13" s="32">
+        <f>SUM(B13:D13)</f>
+        <v>-5.9999999910544917</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="B14" s="32">
+        <f>B5*$B$8</f>
+        <v>0</v>
+      </c>
+      <c r="C14" s="32">
+        <f>C5*$C$8</f>
+        <v>2.5042670826519471</v>
+      </c>
+      <c r="D14" s="32">
+        <f>D5*$D$8</f>
+        <v>0.39658633960356582</v>
+      </c>
+      <c r="F14" s="32">
+        <f>SUM(B14:D14)</f>
+        <v>2.9008534222555129</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="B17" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" s="31">
+        <f>C14+D14</f>
+        <v>2.9008534222555129</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="H23" s="32">
+        <v>1.9999999999999998</v>
+      </c>
+      <c r="I23" s="32">
+        <v>1.3333333673262586</v>
+      </c>
+      <c r="J23" s="32">
+        <v>0.66666665593205843</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:B24"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
     <col min="2" max="2" width="122.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="21" customHeight="1">
+    <row r="1" spans="2:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="25" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="2:2" ht="60" customHeight="1">
+    <row r="2" spans="2:2" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="26" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="2:2" ht="70.2" customHeight="1">
+    <row r="3" spans="2:2" ht="70.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="26" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="2:2" ht="69" customHeight="1">
+    <row r="4" spans="2:2" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="26" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="2:2" ht="100.8" customHeight="1">
+    <row r="5" spans="2:2" ht="100.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="26" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="47.4" customHeight="1">
+    <row r="6" spans="2:2" ht="47.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="26" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="114" customHeight="1">
+    <row r="7" spans="2:2" ht="114" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="26"/>
     </row>
-    <row r="8" spans="2:2" ht="43.2" customHeight="1">
+    <row r="8" spans="2:2" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="26" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="2:2" ht="43.2" customHeight="1">
+    <row r="9" spans="2:2" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="26" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="2:2" ht="78.599999999999994" customHeight="1">
+    <row r="10" spans="2:2" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="26" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="2:2" ht="64.2" customHeight="1">
+    <row r="11" spans="2:2" ht="64.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="26" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="2:2" ht="58.2" customHeight="1">
+    <row r="12" spans="2:2" ht="58.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="26" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="2:2" ht="58.8" customHeight="1">
+    <row r="13" spans="2:2" ht="58.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="26" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="2:2" ht="17.399999999999999">
+    <row r="14" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="B14" s="26"/>
     </row>
-    <row r="15" spans="2:2" ht="17.399999999999999">
+    <row r="15" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="B15" s="26"/>
     </row>
-    <row r="16" spans="2:2" ht="17.399999999999999">
+    <row r="16" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="B16" s="26"/>
     </row>
-    <row r="17" spans="2:2" ht="17.399999999999999">
+    <row r="17" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="B17" s="26"/>
     </row>
-    <row r="18" spans="2:2" ht="17.399999999999999">
+    <row r="18" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="B18" s="26"/>
     </row>
-    <row r="19" spans="2:2" ht="17.399999999999999">
+    <row r="19" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="B19" s="26"/>
     </row>
-    <row r="20" spans="2:2" ht="17.399999999999999">
+    <row r="20" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="B20" s="26"/>
     </row>
-    <row r="21" spans="2:2" ht="17.399999999999999">
+    <row r="21" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B21" s="27"/>
     </row>
-    <row r="22" spans="2:2" ht="17.399999999999999">
+    <row r="22" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B22" s="27"/>
     </row>
-    <row r="23" spans="2:2" ht="17.399999999999999">
+    <row r="23" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B23" s="27"/>
     </row>
-    <row r="24" spans="2:2" ht="17.399999999999999">
+    <row r="24" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B24" s="27"/>
     </row>
   </sheetData>
@@ -4552,8 +7014,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4561,105 +7023,105 @@
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.44140625" customWidth="1"/>
     <col min="2" max="2" width="136.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="21.75" customHeight="1">
+    <row r="1" spans="2:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="28" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="2:2" ht="98.4" customHeight="1">
+    <row r="2" spans="2:2" ht="98.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="26" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="2:2" ht="22.8" customHeight="1">
+    <row r="3" spans="2:2" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="26" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="2:2" ht="82.8" customHeight="1">
+    <row r="4" spans="2:2" ht="82.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="26" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="2:2" ht="68.400000000000006" customHeight="1">
+    <row r="5" spans="2:2" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="26" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="26.4" customHeight="1">
+    <row r="6" spans="2:2" ht="26.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="26" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="98.4" customHeight="1">
+    <row r="7" spans="2:2" ht="98.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="26" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="2:2" ht="67.8" customHeight="1">
+    <row r="8" spans="2:2" ht="67.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="26" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="2:2" ht="46.2" customHeight="1">
+    <row r="9" spans="2:2" ht="46.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="26" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="2:2" ht="97.8" customHeight="1">
+    <row r="10" spans="2:2" ht="97.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="26" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="2:2" ht="60.6" customHeight="1">
+    <row r="11" spans="2:2" ht="60.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="26" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:2" ht="46.8" customHeight="1">
+    <row r="12" spans="2:2" ht="46.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="26" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="2:2" ht="55.2" customHeight="1">
+    <row r="13" spans="2:2" ht="55.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="26" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="2:2" ht="77.400000000000006" customHeight="1">
+    <row r="14" spans="2:2" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="26" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="2:2" ht="46.2" customHeight="1">
+    <row r="15" spans="2:2" ht="46.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="26" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="2:2" ht="46.8" customHeight="1">
+    <row r="16" spans="2:2" ht="46.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="26" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="2:2" ht="17.399999999999999">
+    <row r="17" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="B17" s="26"/>
     </row>
-    <row r="18" spans="2:2" ht="17.399999999999999">
+    <row r="18" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="B18" s="26"/>
     </row>
-    <row r="19" spans="2:2" ht="17.399999999999999">
+    <row r="19" spans="2:2" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="B19" s="26"/>
     </row>
-    <row r="20" spans="2:2">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="14"/>
     </row>
-    <row r="21" spans="2:2">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="14"/>
     </row>
   </sheetData>
@@ -4668,44 +7130,44 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="B4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="B10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B3:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="3.33203125" customWidth="1"/>
     <col min="3" max="3" width="18.33203125" customWidth="1"/>
     <col min="4" max="4" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" ht="33.75" customHeight="1">
+    <row r="3" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="20" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="33" customHeight="1">
+    <row r="6" spans="2:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="17"/>
       <c r="C6" s="13" t="s">
         <v>21</v>
@@ -4714,7 +7176,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="32.25" customHeight="1">
+    <row r="7" spans="2:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="21"/>
       <c r="C7" s="13" t="s">
         <v>23</v>
@@ -4723,7 +7185,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="31.2">
+    <row r="8" spans="2:4" ht="31.2" x14ac:dyDescent="0.25">
       <c r="B8" s="18"/>
       <c r="C8" s="13" t="s">
         <v>25</v>
@@ -4732,7 +7194,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="30" customHeight="1">
+    <row r="9" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="22"/>
       <c r="C9" s="13" t="s">
         <v>27</v>
@@ -4741,7 +7203,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="31.2">
+    <row r="10" spans="2:4" ht="31.2" x14ac:dyDescent="0.25">
       <c r="B10" s="16"/>
       <c r="C10" s="13" t="s">
         <v>29</v>
@@ -4750,7 +7212,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="15.6">
+    <row r="11" spans="2:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="B11" s="23"/>
       <c r="C11" s="13" t="s">
         <v>31</v>
@@ -4764,121 +7226,4 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:B22"/>
-  <sheetViews>
-    <sheetView zoomScale="130" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
-  <cols>
-    <col min="1" max="1" width="1.109375" customWidth="1"/>
-    <col min="2" max="2" width="81" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:2" ht="31.5" customHeight="1">
-      <c r="B1" s="19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="2:2" ht="40.5" customHeight="1">
-      <c r="B2" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2" ht="39.75" customHeight="1">
-      <c r="B3" s="14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" ht="78.75" customHeight="1">
-      <c r="B4" s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" ht="27.75" customHeight="1">
-      <c r="B5" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2" ht="29.25" customHeight="1">
-      <c r="B6" s="14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2" ht="65.25" customHeight="1">
-      <c r="B7" s="14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="2:2" ht="56.25" customHeight="1">
-      <c r="B8" s="14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="2:2" ht="26.25" customHeight="1">
-      <c r="B9" s="14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2" ht="41.25" customHeight="1">
-      <c r="B10" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="2:2" ht="57" customHeight="1">
-      <c r="B11" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="2:2" ht="97.5" customHeight="1">
-      <c r="B12" s="14"/>
-    </row>
-    <row r="13" spans="2:2" ht="28.5" customHeight="1">
-      <c r="B13" s="14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="2:2" ht="51.75" customHeight="1">
-      <c r="B14" s="14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="2:2" ht="31.5" customHeight="1">
-      <c r="B15" s="14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="2:2">
-      <c r="B16" s="14"/>
-    </row>
-    <row r="17" spans="2:2">
-      <c r="B17" s="14"/>
-    </row>
-    <row r="18" spans="2:2">
-      <c r="B18" s="14"/>
-    </row>
-    <row r="19" spans="2:2">
-      <c r="B19" s="14"/>
-    </row>
-    <row r="20" spans="2:2">
-      <c r="B20" s="14"/>
-    </row>
-    <row r="21" spans="2:2">
-      <c r="B21" s="14"/>
-    </row>
-    <row r="22" spans="2:2">
-      <c r="B22" s="14"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <headerFooter alignWithMargins="0"/>
-  <drawing r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>